<commit_message>
Revert "fix issue #i"
This reverts commit 52ae450437f335c605903332a7ff2c2ed771862a.
</commit_message>
<xml_diff>
--- a/doc/Dokumentation.xlsx
+++ b/doc/Dokumentation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Interfaces" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="149">
   <si>
     <t>Interface</t>
   </si>
@@ -868,20 +868,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="11.42578125" style="4"/>
-    <col min="5" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1"/>
+    <col min="4" max="4" width="11.44140625" style="4"/>
+    <col min="5" max="6" width="11.44140625" style="1"/>
+    <col min="7" max="7" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -978,12 +978,6 @@
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:10">
@@ -992,12 +986,6 @@
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -2378,12 +2366,12 @@
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="20.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2513,18 +2501,18 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="14"/>
+    <col min="1" max="1" width="17.5546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="14"/>
     <col min="3" max="4" width="18" style="14" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="13"/>
-    <col min="7" max="7" width="11.5703125" style="12"/>
+    <col min="5" max="5" width="32.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="13"/>
+    <col min="7" max="7" width="11.5546875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1">
@@ -3694,17 +3682,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" style="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="1" max="3" width="11.5546875" style="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="41" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="20"/>
-    <col min="7" max="16384" width="11.5703125" style="1"/>
+    <col min="6" max="6" width="11.5546875" style="20"/>
+    <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4012,10 +4000,10 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>